<commit_message>
Added tests for official net zero peaking
</commit_message>
<xml_diff>
--- a/tests/metadata_indicators_test.xlsx
+++ b/tests/metadata_indicators_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlamboll\ConstrainCode\CarbonBudgetCalculator\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79B0540-02C3-46DD-A479-0FD70BC389EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4655E4FD-8669-4567-9253-45505CE5C39A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29415" yWindow="2280" windowWidth="21930" windowHeight="8970" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="156" yWindow="1536" windowWidth="13824" windowHeight="7176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="categories_indicators_doc_v6" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Category_Vetting_historical</t>
   </si>
@@ -72,12 +72,18 @@
   <si>
     <t>Fine</t>
   </si>
+  <si>
+    <t>year of netzero CO2 emissions</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +105,12 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,12 +152,15 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -8278,7 +8293,7 @@
   <dimension ref="A1:FJ1202"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8317,7 +8332,9 @@
       <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="1"/>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -8483,6 +8500,9 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
+      <c r="L2">
+        <v>2100</v>
+      </c>
       <c r="ER2" s="2"/>
     </row>
     <row r="3" spans="1:166" x14ac:dyDescent="0.3">
@@ -8495,6 +8515,9 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
+      <c r="L3">
+        <v>2050</v>
+      </c>
       <c r="ER3" s="2"/>
     </row>
     <row r="4" spans="1:166" x14ac:dyDescent="0.3">
@@ -8507,6 +8530,9 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
+      <c r="L4" t="s">
+        <v>16</v>
+      </c>
       <c r="ER4" s="2"/>
     </row>
     <row r="5" spans="1:166" x14ac:dyDescent="0.3">
@@ -10046,10 +10072,26 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CA09B611E82E044D956B04788434B279" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="63db924393ce496d7b3c7e8d0fe88ab4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="947e1231-797c-4c4e-88f0-3c2d77cf6589" xmlns:ns3="2ac8e7bc-b8df-4926-831d-c1fd22c8bc48" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dd27cc0c36bdcd4e953137e07af95417" ns2:_="" ns3:_="">
     <xsd:import namespace="947e1231-797c-4c4e-88f0-3c2d77cf6589"/>
@@ -10266,22 +10308,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12306E29-A52D-4220-826A-7F5706A01333}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84D09C26-C5CA-4FF9-BDE3-FB94FA2795D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96685B1E-542D-4CAA-8F58-DDDF61E8638F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10298,21 +10342,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84D09C26-C5CA-4FF9-BDE3-FB94FA2795D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12306E29-A52D-4220-826A-7F5706A01333}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>